<commit_message>
Deals page kind of done
</commit_message>
<xml_diff>
--- a/Prices.xlsx
+++ b/Prices.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach.ZACH-LAPTOP.001\Documents\GitHub\BPASTATE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="27795" windowHeight="13095" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="27795" windowHeight="13095" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Resort" sheetId="1" r:id="rId1"/>
@@ -234,10 +239,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -247,6 +252,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -295,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,7 +338,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -541,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G6"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,14 +622,14 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -681,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,14 +771,14 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -830,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,14 +887,14 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -936,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,14 +1005,14 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1064,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G5"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,14 +1134,14 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1193,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1237,14 +1245,14 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">

</xml_diff>